<commit_message>
Optimization and other adjustments
</commit_message>
<xml_diff>
--- a/Nile_EMODPS_framework/settings/settings_file_Nile.xlsx
+++ b/Nile_EMODPS_framework/settings/settings_file_Nile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasinsari/Documents/master-thesis-project/Nile_EMODPS_framework/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B50DEB-4F35-7742-92F8-DC0011A27CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F5240C-0C12-B447-9A17-8061047EB8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15580" activeTab="1" xr2:uid="{65B2DD87-E74E-094B-8E0A-FAA834E63631}"/>
   </bookViews>
@@ -276,9 +276,6 @@
     <t>[0.60]</t>
   </si>
   <si>
-    <t>[2344]</t>
-  </si>
-  <si>
     <t>[0,0,0, 0,1,0]</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
   </si>
   <si>
     <t>half-an-hour</t>
+  </si>
+  <si>
+    <t>[2544]</t>
   </si>
 </sst>
 </file>
@@ -831,7 +831,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -865,7 +865,7 @@
         <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -879,16 +879,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
         <v>86</v>
-      </c>
-      <c r="D10" t="s">
-        <v>87</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -904,7 +904,7 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,13 +946,13 @@
         <v>58</v>
       </c>
       <c r="B2" s="10">
-        <v>1000000000</v>
+        <v>5000000000</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>77</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="6">
         <v>4571250000</v>
@@ -1295,7 +1295,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -1309,7 +1309,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
         <v>50</v>
@@ -1323,7 +1323,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
         <v>51</v>

</xml_diff>